<commit_message>
Fixed End Moment Formula Corrections
The formulas for partial uniform load and variable loads fixed end moments were incorrect and have been amended as follows:
Cx is a constant of integration and the formulas for slope/cross-section rotation at the ends of a beam for both uniform and variable loads have equivalent definitions meaning the same integration constant order, Where:

EIS at x=0 = C4 
EIS at x=L = -Rr L^2 /2 + C3 L + C6

Rr = right reaction for pin-pin beam
L = beam span
EI are assumed to be constant along the span

To produce equal and opposite end slopes:
-C4 = -ML L/3 + MR L/6
Rr L^2 /2  - C3 L - C6 = ML L/6 - MR L/3

ML = [ Rr L^2 /2  - C3 L - C6 - 2 C4 ] / -1/2 L
MR = [ -C4 + ML L/3] * (6/L)
</commit_message>
<xml_diff>
--- a/01-General Analysis/01 - 3 or 2 Span Beam Moment Distribution.xlsx
+++ b/01-General Analysis/01 - 3 or 2 Span Beam Moment Distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DonB\Desktop\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BB8C1F-0633-48CA-A863-2A5F4DF2D4C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EDCE1A-F658-4857-90E2-3FA3E935287D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95491767-4E54-4AEC-B47C-D53F18FD670B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{95491767-4E54-4AEC-B47C-D53F18FD670B}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="5" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,14 +34,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -58,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="131">
   <si>
     <t>Span 1:</t>
   </si>
@@ -362,9 +360,6 @@
     <t>Right End Delta:</t>
   </si>
   <si>
-    <t>EIS =</t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
@@ -444,16 +439,39 @@
   </si>
   <si>
     <t>OF THIS SOFTWARE, EVEN IF ADVISED OF THE POSSIBILITY OF SUCH DAMAGE.</t>
+  </si>
+  <si>
+    <t>S =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S0 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL = </t>
+  </si>
+  <si>
+    <t>ML,S</t>
+  </si>
+  <si>
+    <t>MR,S</t>
+  </si>
+  <si>
+    <t>E*I =</t>
+  </si>
+  <si>
+    <t>K*ft^2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -532,7 +550,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1002,28 +1020,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1323,26 +1319,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1354,10 +1332,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1391,27 +1369,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
@@ -1425,6 +1382,43 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1742,7 +1736,7 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1753,170 +1747,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="125" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="126"/>
+    </row>
+    <row r="2" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="127"/>
+      <c r="B2" s="128"/>
+    </row>
+    <row r="3" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="127"/>
+      <c r="B3" s="128" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="139"/>
-    </row>
-    <row r="2" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="140"/>
-      <c r="B2" s="141"/>
-    </row>
-    <row r="3" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="140"/>
-      <c r="B3" s="141" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="127"/>
+      <c r="B4" s="128" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="140"/>
-      <c r="B4" s="141" t="s">
+    <row r="5" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="127"/>
+      <c r="B5" s="128"/>
+    </row>
+    <row r="6" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="127"/>
+      <c r="B6" s="128" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="140"/>
-      <c r="B5" s="141"/>
-    </row>
-    <row r="6" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="140"/>
-      <c r="B6" s="141" t="s">
+    <row r="7" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="127"/>
+      <c r="B7" s="128" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="140"/>
-      <c r="B7" s="141" t="s">
+    <row r="8" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="127"/>
+      <c r="B8" s="128"/>
+    </row>
+    <row r="9" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="127"/>
+      <c r="B9" s="128" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="141"/>
-    </row>
-    <row r="9" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="140"/>
-      <c r="B9" s="141" t="s">
+    <row r="10" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="127"/>
+      <c r="B10" s="128" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="140"/>
-      <c r="B10" s="141" t="s">
+    <row r="11" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="127"/>
+      <c r="B11" s="128"/>
+    </row>
+    <row r="12" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="127"/>
+      <c r="B12" s="128" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="140"/>
-      <c r="B11" s="141"/>
-    </row>
-    <row r="12" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
-      <c r="B12" s="141" t="s">
+    <row r="13" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="127"/>
+      <c r="B13" s="128" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="140"/>
-      <c r="B13" s="141" t="s">
+    <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="127"/>
+      <c r="B14" s="128" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="140"/>
-      <c r="B14" s="141" t="s">
+    <row r="15" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="127"/>
+      <c r="B15" s="128"/>
+    </row>
+    <row r="16" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="127"/>
+      <c r="B16" s="128" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="140"/>
-      <c r="B15" s="141"/>
-    </row>
-    <row r="16" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="140"/>
-      <c r="B16" s="141" t="s">
+    <row r="17" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="127"/>
+      <c r="B17" s="128" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="140"/>
-      <c r="B17" s="141" t="s">
+    <row r="18" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="127"/>
+      <c r="B18" s="128" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="140"/>
-      <c r="B18" s="141" t="s">
+    <row r="19" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="127"/>
+      <c r="B19" s="128"/>
+    </row>
+    <row r="20" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="127"/>
+      <c r="B20" s="128" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="140"/>
-      <c r="B19" s="141"/>
-    </row>
-    <row r="20" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="140"/>
-      <c r="B20" s="141" t="s">
+    <row r="21" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="127"/>
+      <c r="B21" s="128" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="140"/>
-      <c r="B21" s="141" t="s">
+    <row r="22" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="127"/>
+      <c r="B22" s="128" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="140"/>
-      <c r="B22" s="141" t="s">
+    <row r="23" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="127"/>
+      <c r="B23" s="128" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="140"/>
-      <c r="B23" s="141" t="s">
+    <row r="24" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="127"/>
+      <c r="B24" s="128" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="140"/>
-      <c r="B24" s="141" t="s">
+    <row r="25" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="127"/>
+      <c r="B25" s="128" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="140"/>
-      <c r="B25" s="141" t="s">
+    <row r="26" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="127"/>
+      <c r="B26" s="128" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="140"/>
-      <c r="B26" s="141" t="s">
+    <row r="27" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="127"/>
+      <c r="B27" s="128" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="140"/>
-      <c r="B27" s="141" t="s">
+    <row r="28" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="127"/>
+      <c r="B28" s="128" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="140"/>
-      <c r="B28" s="141" t="s">
+    <row r="29" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="127"/>
+      <c r="B29" s="128" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="140"/>
-      <c r="B29" s="141" t="s">
-        <v>124</v>
-      </c>
-    </row>
     <row r="30" spans="1:2" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="142"/>
-      <c r="B30" s="143"/>
+      <c r="A30" s="129"/>
+      <c r="B30" s="130"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1929,8 +1923,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q113"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,7 +1943,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1979,32 +1973,32 @@
         <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>30.8</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
         <f>D4*144</f>
-        <v>4176</v>
+        <v>144</v>
       </c>
       <c r="G4">
         <f>E4/POWER(12,4)</f>
-        <v>1.4853395061728396E-3</v>
+        <v>4.8225308641975306E-5</v>
       </c>
       <c r="H4" s="1">
         <f>(F4*G4)/B4</f>
-        <v>0.62027777777777782</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="I4" s="1">
         <f>IF(B9=0,(0.75*F4*G4)/B4,(F4*G4)/B4)</f>
-        <v>0.46520833333333333</v>
+        <v>2.6041666666666665E-3</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2012,32 +2006,32 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>30.8</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:F6" si="0">D5*144</f>
-        <v>4176</v>
+        <v>144</v>
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G6" si="1">E5/POWER(12,4)</f>
-        <v>1.4853395061728396E-3</v>
+        <v>4.8225308641975306E-5</v>
       </c>
       <c r="H5" s="1">
         <f>(F5*G5)/B5</f>
-        <v>0.62027777777777782</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="I5" s="1">
         <f>H5</f>
-        <v>0.62027777777777782</v>
+        <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -2045,32 +2039,32 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>30.8</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>4176</v>
+        <v>144</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>1.4853395061728396E-3</v>
+        <v>4.8225308641975306E-5</v>
       </c>
       <c r="H6" s="1">
         <f>IF(B10=0,(0.75*F6*G6)/B6,(F6*G6)/B6)</f>
-        <v>0.46520833333333333</v>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="I6" s="1">
         <f>(F6*G6)/B6</f>
-        <v>0.62027777777777782</v>
+        <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -2120,7 +2114,7 @@
         <v>35</v>
       </c>
       <c r="K12" s="80"/>
-      <c r="L12" s="119"/>
+      <c r="L12" s="113"/>
       <c r="M12" s="80"/>
       <c r="N12" s="80"/>
       <c r="O12" s="80"/>
@@ -2136,10 +2130,10 @@
         <v>24</v>
       </c>
       <c r="K13" s="80"/>
-      <c r="L13" s="119"/>
+      <c r="L13" s="113"/>
       <c r="M13" s="80"/>
       <c r="N13" s="80"/>
-      <c r="O13" s="119"/>
+      <c r="O13" s="113"/>
       <c r="P13" s="80"/>
       <c r="Q13" s="80"/>
     </row>
@@ -2167,35 +2161,35 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="11">
+      <c r="B15" s="142">
         <f>B84</f>
         <v>0</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="142">
         <f t="shared" ref="C15:G15" si="2">C84</f>
-        <v>9.9960000000328399</v>
-      </c>
-      <c r="D15" s="11">
+        <v>5.5509328580574689E-5</v>
+      </c>
+      <c r="D15" s="142">
         <f t="shared" si="2"/>
-        <v>-9.9959999999781104</v>
-      </c>
-      <c r="E15" s="11">
+        <v>-5.5509328579206947E-5</v>
+      </c>
+      <c r="E15" s="142">
         <f t="shared" si="2"/>
-        <v>9.9959999999781104</v>
-      </c>
-      <c r="F15" s="11">
+        <v>-1.3877332144801735E-5</v>
+      </c>
+      <c r="F15" s="142">
         <f t="shared" si="2"/>
-        <v>-9.9960000000328399</v>
-      </c>
-      <c r="G15" s="11">
+        <v>1.3877332144801739E-5</v>
+      </c>
+      <c r="G15" s="142">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K15" s="80"/>
-      <c r="L15" s="120"/>
-      <c r="M15" s="120"/>
-      <c r="N15" s="120"/>
-      <c r="O15" s="120"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
+      <c r="N15" s="114"/>
+      <c r="O15" s="114"/>
       <c r="P15" s="80"/>
       <c r="Q15" s="80"/>
     </row>
@@ -2235,12 +2229,12 @@
       <c r="G18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="121"/>
-      <c r="L18" s="122"/>
+      <c r="K18" s="115"/>
+      <c r="L18" s="116"/>
       <c r="M18" s="131"/>
       <c r="N18" s="131"/>
-      <c r="O18" s="122"/>
-      <c r="P18" s="123"/>
+      <c r="O18" s="116"/>
+      <c r="P18" s="117"/>
       <c r="Q18" s="80"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2265,12 +2259,12 @@
       <c r="G19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="121"/>
-      <c r="L19" s="122"/>
-      <c r="M19" s="124"/>
-      <c r="N19" s="122"/>
-      <c r="O19" s="122"/>
-      <c r="P19" s="122"/>
+      <c r="K19" s="115"/>
+      <c r="L19" s="116"/>
+      <c r="M19" s="118"/>
+      <c r="N19" s="116"/>
+      <c r="O19" s="116"/>
+      <c r="P19" s="116"/>
       <c r="Q19" s="80"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2279,34 +2273,34 @@
       </c>
       <c r="B20" s="8">
         <f>H4</f>
-        <v>0.62027777777777782</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="C20" s="4">
         <f>I4</f>
-        <v>0.46520833333333333</v>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="D20" s="5">
         <f>H5</f>
-        <v>0.62027777777777782</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="E20" s="9">
         <f>I5</f>
-        <v>0.62027777777777782</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="F20" s="9">
         <f>H6</f>
-        <v>0.46520833333333333</v>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="G20" s="10">
         <f>I6</f>
-        <v>0.62027777777777782</v>
-      </c>
-      <c r="K20" s="121"/>
-      <c r="L20" s="120"/>
-      <c r="M20" s="120"/>
-      <c r="N20" s="120"/>
-      <c r="O20" s="120"/>
-      <c r="P20" s="120"/>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="K20" s="115"/>
+      <c r="L20" s="114"/>
+      <c r="M20" s="114"/>
+      <c r="N20" s="114"/>
+      <c r="O20" s="114"/>
+      <c r="P20" s="114"/>
       <c r="Q20" s="80"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2319,30 +2313,30 @@
       </c>
       <c r="C21" s="4">
         <f>C20/(C20+D20)</f>
-        <v>0.42857142857142855</v>
+        <v>0.4285714285714286</v>
       </c>
       <c r="D21" s="5">
         <f>D20/(C20+D20)</f>
-        <v>0.5714285714285714</v>
+        <v>0.57142857142857151</v>
       </c>
       <c r="E21" s="9">
         <f>E20/(E20+F20)</f>
-        <v>0.5714285714285714</v>
+        <v>0.57142857142857151</v>
       </c>
       <c r="F21" s="9">
         <f>F20/(E20+F20)</f>
-        <v>0.42857142857142855</v>
+        <v>0.4285714285714286</v>
       </c>
       <c r="G21" s="10">
         <f>IF(B10=0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="K21" s="121"/>
-      <c r="L21" s="120"/>
-      <c r="M21" s="120"/>
-      <c r="N21" s="120"/>
-      <c r="O21" s="120"/>
-      <c r="P21" s="120"/>
+      <c r="K21" s="115"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="114"/>
+      <c r="N21" s="114"/>
+      <c r="O21" s="114"/>
+      <c r="P21" s="114"/>
       <c r="Q21" s="80"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2371,12 +2365,12 @@
         <f>IF(B10=0,0.5,0)</f>
         <v>0.5</v>
       </c>
-      <c r="K22" s="121"/>
-      <c r="L22" s="120"/>
-      <c r="M22" s="120"/>
-      <c r="N22" s="120"/>
-      <c r="O22" s="120"/>
-      <c r="P22" s="120"/>
+      <c r="K22" s="115"/>
+      <c r="L22" s="114"/>
+      <c r="M22" s="114"/>
+      <c r="N22" s="114"/>
+      <c r="O22" s="114"/>
+      <c r="P22" s="114"/>
       <c r="Q22" s="80"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2384,25 +2378,25 @@
         <v>20</v>
       </c>
       <c r="B23" s="33">
-        <v>-8.33</v>
+        <v>2.0815998217476152E-4</v>
       </c>
       <c r="C23" s="34">
-        <v>8.33</v>
+        <v>2.0815998217476152E-4</v>
       </c>
       <c r="D23" s="35">
-        <v>-8.33</v>
+        <v>0</v>
       </c>
       <c r="E23" s="36">
-        <v>8.33</v>
+        <v>0</v>
       </c>
       <c r="F23" s="36">
-        <v>-8.33</v>
+        <v>0</v>
       </c>
       <c r="G23" s="37">
-        <v>8.33</v>
+        <v>0</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="K23" s="121"/>
+      <c r="K23" s="115"/>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
       <c r="N23" s="28"/>
@@ -2416,27 +2410,27 @@
       </c>
       <c r="B24" s="16">
         <f>-1*B23*$B$21</f>
-        <v>8.33</v>
+        <v>-2.0815998217476152E-4</v>
       </c>
       <c r="C24" s="17">
         <f>B24*$B$22</f>
-        <v>4.165</v>
+        <v>-1.0407999108738076E-4</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="17"/>
       <c r="F24" s="18">
         <f>G24*$G$22</f>
-        <v>-4.165</v>
+        <v>0</v>
       </c>
       <c r="G24" s="19">
         <f>-1*G23*$G$21</f>
-        <v>-8.33</v>
+        <v>0</v>
       </c>
       <c r="K24" s="80"/>
-      <c r="L24" s="125"/>
-      <c r="M24" s="125"/>
-      <c r="N24" s="125"/>
-      <c r="O24" s="125"/>
+      <c r="L24" s="119"/>
+      <c r="M24" s="119"/>
+      <c r="N24" s="119"/>
+      <c r="O24" s="119"/>
       <c r="P24" s="80"/>
       <c r="Q24" s="80"/>
     </row>
@@ -2444,26 +2438,26 @@
       <c r="B25" s="16"/>
       <c r="C25" s="17">
         <f>SUM(C$23:D24)*$C$21*-1</f>
-        <v>-1.7849999999999999</v>
+        <v>-4.4605710466020329E-5</v>
       </c>
       <c r="D25" s="18">
         <f>SUM(C$23:D24)*$D$21*-1</f>
-        <v>-2.38</v>
+        <v>-5.9474280621360445E-5</v>
       </c>
       <c r="E25" s="17">
         <f>SUM(E$23:F24)*$E$21*-1</f>
-        <v>2.38</v>
+        <v>0</v>
       </c>
       <c r="F25" s="18">
         <f>SUM(E$23:F24)*$F$21*-1</f>
-        <v>1.7849999999999999</v>
+        <v>0</v>
       </c>
       <c r="G25" s="19"/>
       <c r="K25" s="80"/>
-      <c r="L25" s="125"/>
-      <c r="M25" s="125"/>
-      <c r="N25" s="125"/>
-      <c r="O25" s="125"/>
+      <c r="L25" s="119"/>
+      <c r="M25" s="119"/>
+      <c r="N25" s="119"/>
+      <c r="O25" s="119"/>
       <c r="P25" s="80"/>
       <c r="Q25" s="80"/>
     </row>
@@ -2475,11 +2469,11 @@
       <c r="C26" s="17"/>
       <c r="D26" s="18">
         <f>E25*$E$22</f>
-        <v>1.19</v>
+        <v>0</v>
       </c>
       <c r="E26" s="17">
         <f>D25*$D$22</f>
-        <v>-1.19</v>
+        <v>-2.9737140310680223E-5</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="19">
@@ -2487,10 +2481,10 @@
         <v>0</v>
       </c>
       <c r="K26" s="80"/>
-      <c r="L26" s="125"/>
-      <c r="M26" s="125"/>
-      <c r="N26" s="125"/>
-      <c r="O26" s="125"/>
+      <c r="L26" s="119"/>
+      <c r="M26" s="119"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="119"/>
       <c r="P26" s="80"/>
       <c r="Q26" s="80"/>
     </row>
@@ -2517,10 +2511,10 @@
         <v>0</v>
       </c>
       <c r="K27" s="80"/>
-      <c r="L27" s="125"/>
-      <c r="M27" s="125"/>
-      <c r="N27" s="125"/>
-      <c r="O27" s="125"/>
+      <c r="L27" s="119"/>
+      <c r="M27" s="119"/>
+      <c r="N27" s="119"/>
+      <c r="O27" s="119"/>
       <c r="P27" s="80"/>
       <c r="Q27" s="80"/>
     </row>
@@ -2528,26 +2522,26 @@
       <c r="B28" s="20"/>
       <c r="C28" s="21">
         <f>SUM(C$23:D27)*$C$21*-1</f>
-        <v>-0.5099999999999999</v>
+        <v>5.8082259240294885E-21</v>
       </c>
       <c r="D28" s="22">
         <f>SUM(C$23:D27)*$D$21*-1</f>
-        <v>-0.67999999999999994</v>
+        <v>7.7443012320393185E-21</v>
       </c>
       <c r="E28" s="21">
         <f>SUM(E$23:F27)*$E$21*-1</f>
-        <v>0.68</v>
+        <v>1.6992651606102987E-5</v>
       </c>
       <c r="F28" s="22">
         <f>SUM(E$23:F27)*$F$21*-1</f>
-        <v>0.51</v>
+        <v>1.2744488704577239E-5</v>
       </c>
       <c r="G28" s="23"/>
       <c r="K28" s="80"/>
-      <c r="L28" s="125"/>
-      <c r="M28" s="125"/>
-      <c r="N28" s="125"/>
-      <c r="O28" s="125"/>
+      <c r="L28" s="119"/>
+      <c r="M28" s="119"/>
+      <c r="N28" s="119"/>
+      <c r="O28" s="119"/>
       <c r="P28" s="80"/>
       <c r="Q28" s="80"/>
     </row>
@@ -2559,11 +2553,11 @@
       <c r="C29" s="21"/>
       <c r="D29" s="22">
         <f>E28*$E$22</f>
-        <v>0.34</v>
+        <v>8.4963258030514936E-6</v>
       </c>
       <c r="E29" s="21">
         <f>D28*$D$22</f>
-        <v>-0.33999999999999997</v>
+        <v>3.8721506160196592E-21</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="23">
@@ -2571,10 +2565,10 @@
         <v>0</v>
       </c>
       <c r="K29" s="80"/>
-      <c r="L29" s="125"/>
-      <c r="M29" s="125"/>
-      <c r="N29" s="125"/>
-      <c r="O29" s="125"/>
+      <c r="L29" s="119"/>
+      <c r="M29" s="119"/>
+      <c r="N29" s="119"/>
+      <c r="O29" s="119"/>
       <c r="P29" s="80"/>
       <c r="Q29" s="80"/>
     </row>
@@ -2601,10 +2595,10 @@
         <v>0</v>
       </c>
       <c r="K30" s="80"/>
-      <c r="L30" s="125"/>
-      <c r="M30" s="125"/>
-      <c r="N30" s="125"/>
-      <c r="O30" s="125"/>
+      <c r="L30" s="119"/>
+      <c r="M30" s="119"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="119"/>
       <c r="P30" s="80"/>
       <c r="Q30" s="80"/>
     </row>
@@ -2612,26 +2606,26 @@
       <c r="B31" s="16"/>
       <c r="C31" s="17">
         <f>SUM(C$23:D30)*$C$21*-1</f>
-        <v>-0.14571428571428577</v>
+        <v>-3.6412824870220689E-6</v>
       </c>
       <c r="D31" s="18">
         <f>SUM(C$23:D30)*$D$21*-1</f>
-        <v>-0.19428571428571434</v>
+        <v>-4.855043316029426E-6</v>
       </c>
       <c r="E31" s="17">
         <f>SUM(E$23:F30)*$E$21*-1</f>
-        <v>0.19428571428571431</v>
+        <v>-4.1487328028782073E-21</v>
       </c>
       <c r="F31" s="18">
         <f>SUM(E$23:F30)*$F$21*-1</f>
-        <v>0.14571428571428574</v>
+        <v>-3.1115496021586551E-21</v>
       </c>
       <c r="G31" s="19"/>
       <c r="K31" s="80"/>
-      <c r="L31" s="125"/>
-      <c r="M31" s="125"/>
-      <c r="N31" s="125"/>
-      <c r="O31" s="125"/>
+      <c r="L31" s="119"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="119"/>
       <c r="P31" s="80"/>
       <c r="Q31" s="80"/>
     </row>
@@ -2643,11 +2637,11 @@
       <c r="C32" s="17"/>
       <c r="D32" s="18">
         <f>E31*$E$22</f>
-        <v>9.7142857142857156E-2</v>
+        <v>-2.0743664014391037E-21</v>
       </c>
       <c r="E32" s="17">
         <f>D31*$D$22</f>
-        <v>-9.714285714285717E-2</v>
+        <v>-2.427521658014713E-6</v>
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="19">
@@ -2655,10 +2649,10 @@
         <v>0</v>
       </c>
       <c r="K32" s="80"/>
-      <c r="L32" s="125"/>
-      <c r="M32" s="125"/>
-      <c r="N32" s="125"/>
-      <c r="O32" s="125"/>
+      <c r="L32" s="119"/>
+      <c r="M32" s="119"/>
+      <c r="N32" s="119"/>
+      <c r="O32" s="119"/>
       <c r="P32" s="80"/>
       <c r="Q32" s="80"/>
     </row>
@@ -2685,10 +2679,10 @@
         <v>0</v>
       </c>
       <c r="K33" s="80"/>
-      <c r="L33" s="125"/>
-      <c r="M33" s="125"/>
-      <c r="N33" s="125"/>
-      <c r="O33" s="125"/>
+      <c r="L33" s="119"/>
+      <c r="M33" s="119"/>
+      <c r="N33" s="119"/>
+      <c r="O33" s="119"/>
       <c r="P33" s="80"/>
       <c r="Q33" s="80"/>
     </row>
@@ -2696,26 +2690,26 @@
       <c r="B34" s="20"/>
       <c r="C34" s="21">
         <f>SUM(C$23:D33)*$C$21*-1</f>
-        <v>-4.1632653061224503E-2</v>
+        <v>1.2520282922971733E-21</v>
       </c>
       <c r="D34" s="22">
         <f>SUM(C$23:D33)*$D$21*-1</f>
-        <v>-5.5510204081632673E-2</v>
+        <v>1.6693710563962311E-21</v>
       </c>
       <c r="E34" s="21">
         <f>SUM(E$23:F33)*$E$21*-1</f>
-        <v>5.551020408163268E-2</v>
+        <v>1.3871552331512648E-6</v>
       </c>
       <c r="F34" s="22">
         <f>SUM(E$23:F33)*$F$21*-1</f>
-        <v>4.163265306122451E-2</v>
+        <v>1.0403664248634484E-6</v>
       </c>
       <c r="G34" s="23"/>
       <c r="K34" s="80"/>
-      <c r="L34" s="125"/>
-      <c r="M34" s="125"/>
-      <c r="N34" s="125"/>
-      <c r="O34" s="125"/>
+      <c r="L34" s="119"/>
+      <c r="M34" s="119"/>
+      <c r="N34" s="119"/>
+      <c r="O34" s="119"/>
       <c r="P34" s="80"/>
       <c r="Q34" s="80"/>
     </row>
@@ -2727,11 +2721,11 @@
       <c r="C35" s="21"/>
       <c r="D35" s="22">
         <f>E34*$E$22</f>
-        <v>2.775510204081634E-2</v>
+        <v>6.935776165756324E-7</v>
       </c>
       <c r="E35" s="21">
         <f>D34*$D$22</f>
-        <v>-2.7755102040816337E-2</v>
+        <v>8.3468552819811554E-22</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="23">
@@ -2739,10 +2733,10 @@
         <v>0</v>
       </c>
       <c r="K35" s="80"/>
-      <c r="L35" s="125"/>
-      <c r="M35" s="125"/>
-      <c r="N35" s="125"/>
-      <c r="O35" s="125"/>
+      <c r="L35" s="119"/>
+      <c r="M35" s="119"/>
+      <c r="N35" s="119"/>
+      <c r="O35" s="119"/>
       <c r="P35" s="80"/>
       <c r="Q35" s="80"/>
     </row>
@@ -2769,10 +2763,10 @@
         <v>0</v>
       </c>
       <c r="K36" s="80"/>
-      <c r="L36" s="125"/>
-      <c r="M36" s="125"/>
-      <c r="N36" s="125"/>
-      <c r="O36" s="125"/>
+      <c r="L36" s="119"/>
+      <c r="M36" s="119"/>
+      <c r="N36" s="119"/>
+      <c r="O36" s="119"/>
       <c r="P36" s="80"/>
       <c r="Q36" s="80"/>
     </row>
@@ -2780,26 +2774,26 @@
       <c r="B37" s="16"/>
       <c r="C37" s="17">
         <f>SUM(C$23:D36)*$C$21*-1</f>
-        <v>-1.1895043731778434E-2</v>
+        <v>-2.9724754996098534E-7</v>
       </c>
       <c r="D37" s="18">
         <f>SUM(C$23:D36)*$D$21*-1</f>
-        <v>-1.5860058309037913E-2</v>
+        <v>-3.9633006661464716E-7</v>
       </c>
       <c r="E37" s="17">
         <f>SUM(E$23:F36)*$E$21*-1</f>
-        <v>1.586005830903791E-2</v>
+        <v>-5.9796786572096612E-22</v>
       </c>
       <c r="F37" s="18">
         <f>SUM(E$23:F36)*$F$21*-1</f>
-        <v>1.1895043731778432E-2</v>
+        <v>-4.4847589929072459E-22</v>
       </c>
       <c r="G37" s="19"/>
       <c r="K37" s="80"/>
-      <c r="L37" s="125"/>
-      <c r="M37" s="125"/>
-      <c r="N37" s="125"/>
-      <c r="O37" s="125"/>
+      <c r="L37" s="119"/>
+      <c r="M37" s="119"/>
+      <c r="N37" s="119"/>
+      <c r="O37" s="119"/>
       <c r="P37" s="80"/>
       <c r="Q37" s="80"/>
     </row>
@@ -2811,11 +2805,11 @@
       <c r="C38" s="17"/>
       <c r="D38" s="18">
         <f>E37*$E$22</f>
-        <v>7.9300291545189548E-3</v>
+        <v>-2.9898393286048306E-22</v>
       </c>
       <c r="E38" s="17">
         <f>D37*$D$22</f>
-        <v>-7.9300291545189566E-3</v>
+        <v>-1.9816503330732358E-7</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="19">
@@ -2823,10 +2817,10 @@
         <v>0</v>
       </c>
       <c r="K38" s="80"/>
-      <c r="L38" s="125"/>
-      <c r="M38" s="125"/>
-      <c r="N38" s="125"/>
-      <c r="O38" s="125"/>
+      <c r="L38" s="119"/>
+      <c r="M38" s="119"/>
+      <c r="N38" s="119"/>
+      <c r="O38" s="119"/>
       <c r="P38" s="80"/>
       <c r="Q38" s="80"/>
     </row>
@@ -2853,10 +2847,10 @@
         <v>0</v>
       </c>
       <c r="K39" s="80"/>
-      <c r="L39" s="125"/>
-      <c r="M39" s="125"/>
-      <c r="N39" s="125"/>
-      <c r="O39" s="125"/>
+      <c r="L39" s="119"/>
+      <c r="M39" s="119"/>
+      <c r="N39" s="119"/>
+      <c r="O39" s="119"/>
       <c r="P39" s="80"/>
       <c r="Q39" s="80"/>
     </row>
@@ -2864,26 +2858,26 @@
       <c r="B40" s="20"/>
       <c r="C40" s="21">
         <f>SUM(C$23:D39)*$C$21*-1</f>
-        <v>-3.3985839233652664E-3</v>
+        <v>1.7351273625740171E-22</v>
       </c>
       <c r="D40" s="22">
         <f>SUM(C$23:D39)*$D$21*-1</f>
-        <v>-4.5314452311536885E-3</v>
+        <v>2.3135031500986896E-22</v>
       </c>
       <c r="E40" s="21">
         <f>SUM(E$23:F39)*$E$21*-1</f>
-        <v>4.5314452311536902E-3</v>
+        <v>1.1323716188989921E-7</v>
       </c>
       <c r="F40" s="22">
         <f>SUM(E$23:F39)*$F$21*-1</f>
-        <v>3.3985839233652677E-3</v>
+        <v>8.4927871417424401E-8</v>
       </c>
       <c r="G40" s="23"/>
       <c r="K40" s="80"/>
-      <c r="L40" s="125"/>
-      <c r="M40" s="125"/>
-      <c r="N40" s="125"/>
-      <c r="O40" s="125"/>
+      <c r="L40" s="119"/>
+      <c r="M40" s="119"/>
+      <c r="N40" s="119"/>
+      <c r="O40" s="119"/>
       <c r="P40" s="80"/>
       <c r="Q40" s="80"/>
     </row>
@@ -2895,11 +2889,11 @@
       <c r="C41" s="21"/>
       <c r="D41" s="22">
         <f>E40*$E$22</f>
-        <v>2.2657226155768451E-3</v>
+        <v>5.6618580944949603E-8</v>
       </c>
       <c r="E41" s="21">
         <f>D40*$D$22</f>
-        <v>-2.2657226155768442E-3</v>
+        <v>1.1567515750493448E-22</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="23">
@@ -2907,10 +2901,10 @@
         <v>0</v>
       </c>
       <c r="K41" s="80"/>
-      <c r="L41" s="125"/>
-      <c r="M41" s="125"/>
-      <c r="N41" s="125"/>
-      <c r="O41" s="125"/>
+      <c r="L41" s="119"/>
+      <c r="M41" s="119"/>
+      <c r="N41" s="119"/>
+      <c r="O41" s="119"/>
       <c r="P41" s="80"/>
       <c r="Q41" s="80"/>
     </row>
@@ -2937,10 +2931,10 @@
         <v>0</v>
       </c>
       <c r="K42" s="80"/>
-      <c r="L42" s="125"/>
-      <c r="M42" s="125"/>
-      <c r="N42" s="125"/>
-      <c r="O42" s="125"/>
+      <c r="L42" s="119"/>
+      <c r="M42" s="119"/>
+      <c r="N42" s="119"/>
+      <c r="O42" s="119"/>
       <c r="P42" s="80"/>
       <c r="Q42" s="80"/>
     </row>
@@ -2948,26 +2942,26 @@
       <c r="B43" s="16"/>
       <c r="C43" s="17">
         <f>SUM(C$23:D42)*$C$21*-1</f>
-        <v>-9.7102397810436216E-4</v>
+        <v>-2.4265106119264118E-8</v>
       </c>
       <c r="D43" s="18">
         <f>SUM(C$23:D42)*$D$21*-1</f>
-        <v>-1.2946986374724829E-3</v>
+        <v>-3.2353474825685491E-8</v>
       </c>
       <c r="E43" s="17">
         <f>SUM(E$23:F42)*$E$21*-1</f>
-        <v>1.2946986374724825E-3</v>
+        <v>-8.1225678346646504E-23</v>
       </c>
       <c r="F43" s="18">
         <f>SUM(E$23:F42)*$F$21*-1</f>
-        <v>9.7102397810436194E-4</v>
+        <v>-6.0919258759984875E-23</v>
       </c>
       <c r="G43" s="19"/>
       <c r="K43" s="80"/>
-      <c r="L43" s="125"/>
-      <c r="M43" s="125"/>
-      <c r="N43" s="125"/>
-      <c r="O43" s="125"/>
+      <c r="L43" s="119"/>
+      <c r="M43" s="119"/>
+      <c r="N43" s="119"/>
+      <c r="O43" s="119"/>
       <c r="P43" s="80"/>
       <c r="Q43" s="80"/>
     </row>
@@ -2979,11 +2973,11 @@
       <c r="C44" s="17"/>
       <c r="D44" s="18">
         <f>E43*$E$22</f>
-        <v>6.4734931873624126E-4</v>
+        <v>-4.0612839173323252E-23</v>
       </c>
       <c r="E44" s="17">
         <f>D43*$D$22</f>
-        <v>-6.4734931873624147E-4</v>
+        <v>-1.6176737412842746E-8</v>
       </c>
       <c r="F44" s="18"/>
       <c r="G44" s="19">
@@ -2991,10 +2985,10 @@
         <v>0</v>
       </c>
       <c r="K44" s="80"/>
-      <c r="L44" s="125"/>
-      <c r="M44" s="125"/>
-      <c r="N44" s="125"/>
-      <c r="O44" s="125"/>
+      <c r="L44" s="119"/>
+      <c r="M44" s="119"/>
+      <c r="N44" s="119"/>
+      <c r="O44" s="119"/>
       <c r="P44" s="80"/>
       <c r="Q44" s="80"/>
     </row>
@@ -3032,19 +3026,19 @@
       <c r="B46" s="20"/>
       <c r="C46" s="21">
         <f>SUM(C$23:D45)*$C$21*-1</f>
-        <v>-2.7743542231553197E-4</v>
+        <v>2.0241550317320348E-23</v>
       </c>
       <c r="D46" s="22">
         <f>SUM(C$23:D45)*$D$21*-1</f>
-        <v>-3.6991389642070929E-4</v>
+        <v>2.6988733756427129E-23</v>
       </c>
       <c r="E46" s="21">
         <f>SUM(E$23:F45)*$E$21*-1</f>
-        <v>3.6991389642070951E-4</v>
+        <v>9.2438499501958558E-9</v>
       </c>
       <c r="F46" s="22">
         <f>SUM(E$23:F45)*$F$21*-1</f>
-        <v>2.7743542231553213E-4</v>
+        <v>6.9328874626468914E-9</v>
       </c>
       <c r="G46" s="23"/>
       <c r="K46" s="80"/>
@@ -3063,11 +3057,11 @@
       <c r="C47" s="21"/>
       <c r="D47" s="22">
         <f>E46*$E$22</f>
-        <v>1.8495694821035475E-4</v>
+        <v>4.6219249750979279E-9</v>
       </c>
       <c r="E47" s="21">
         <f>D46*$D$22</f>
-        <v>-1.8495694821035464E-4</v>
+        <v>1.3494366878213564E-23</v>
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="23">
@@ -3109,19 +3103,19 @@
       <c r="B49" s="16"/>
       <c r="C49" s="17">
         <f>SUM(C$23:D48)*$C$21*-1</f>
-        <v>-7.9267263518723456E-5</v>
+        <v>-1.9808249893276836E-9</v>
       </c>
       <c r="D49" s="18">
         <f>SUM(C$23:D48)*$D$21*-1</f>
-        <v>-1.0568968469163128E-4</v>
+        <v>-2.6410999857702447E-9</v>
       </c>
       <c r="E49" s="17">
         <f>SUM(E$23:F48)*$E$21*-1</f>
-        <v>1.0568968469163126E-4</v>
+        <v>-8.6564160590397843E-24</v>
       </c>
       <c r="F49" s="18">
         <f>SUM(E$23:F48)*$F$21*-1</f>
-        <v>7.9267263518723442E-5</v>
+        <v>-6.4923120442798375E-24</v>
       </c>
       <c r="G49" s="19"/>
     </row>
@@ -3133,11 +3127,11 @@
       <c r="C50" s="17"/>
       <c r="D50" s="18">
         <f>E49*$E$22</f>
-        <v>5.2844842345815628E-5</v>
+        <v>-4.3282080295198922E-24</v>
       </c>
       <c r="E50" s="17">
         <f>D49*$D$22</f>
-        <v>-5.2844842345815642E-5</v>
+        <v>-1.3205499928851223E-9</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="19">
@@ -3172,19 +3166,19 @@
       <c r="B52" s="20"/>
       <c r="C52" s="21">
         <f>SUM(C$23:D51)*$C$21*-1</f>
-        <v>-2.2647789576778131E-5</v>
+        <v>2.0321992867698884E-24</v>
       </c>
       <c r="D52" s="22">
         <f>SUM(C$23:D51)*$D$21*-1</f>
-        <v>-3.0197052769037508E-5</v>
+        <v>2.7095990490265179E-24</v>
       </c>
       <c r="E52" s="21">
         <f>SUM(E$23:F51)*$E$21*-1</f>
-        <v>3.0197052769037508E-5</v>
+        <v>7.5459999593435576E-10</v>
       </c>
       <c r="F52" s="22">
         <f>SUM(E$23:F51)*$F$21*-1</f>
-        <v>2.2647789576778131E-5</v>
+        <v>5.6594999695076679E-10</v>
       </c>
       <c r="G52" s="23"/>
     </row>
@@ -3196,11 +3190,11 @@
       <c r="C53" s="21"/>
       <c r="D53" s="22">
         <f>E52*$E$22</f>
-        <v>1.5098526384518754E-5</v>
+        <v>3.7729999796717788E-10</v>
       </c>
       <c r="E53" s="21">
         <f>D52*$D$22</f>
-        <v>-1.5098526384518754E-5</v>
+        <v>1.354799524513259E-24</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="23">
@@ -3235,19 +3229,19 @@
       <c r="B55" s="16"/>
       <c r="C55" s="17">
         <f>SUM(C$23:D54)*$C$21*-1</f>
-        <v>-6.4707970219366101E-6</v>
+        <v>-1.6169999912879052E-10</v>
       </c>
       <c r="D55" s="18">
         <f>SUM(C$23:D54)*$D$21*-1</f>
-        <v>-8.6277293625821463E-6</v>
+        <v>-2.1559999883838738E-10</v>
       </c>
       <c r="E55" s="17">
         <f>SUM(E$23:F54)*$E$21*-1</f>
-        <v>8.6277293625821463E-6</v>
+        <v>-8.923398158008664E-25</v>
       </c>
       <c r="F55" s="18">
         <f>SUM(E$23:F54)*$F$21*-1</f>
-        <v>6.4707970219366101E-6</v>
+        <v>-6.6925486185064975E-25</v>
       </c>
       <c r="G55" s="19"/>
     </row>
@@ -3259,11 +3253,11 @@
       <c r="C56" s="17"/>
       <c r="D56" s="18">
         <f>E55*$E$22</f>
-        <v>4.3138646812910731E-6</v>
+        <v>-4.461699079004332E-25</v>
       </c>
       <c r="E56" s="17">
         <f>D55*$D$22</f>
-        <v>-4.3138646812910731E-6</v>
+        <v>-1.0779999941919369E-10</v>
       </c>
       <c r="F56" s="18"/>
       <c r="G56" s="19">
@@ -3298,19 +3292,19 @@
       <c r="B58" s="20"/>
       <c r="C58" s="21">
         <f>SUM(C$23:D57)*$C$21*-1</f>
-        <v>-1.8487991491247463E-6</v>
+        <v>2.0229398658973516E-25</v>
       </c>
       <c r="D58" s="22">
         <f>SUM(C$23:D57)*$D$21*-1</f>
-        <v>-2.4650655321663283E-6</v>
+        <v>2.6972531545298023E-25</v>
       </c>
       <c r="E58" s="21">
         <f>SUM(E$23:F57)*$E$21*-1</f>
-        <v>2.4650655321663279E-6</v>
+        <v>6.1599999668110684E-11</v>
       </c>
       <c r="F58" s="22">
         <f>SUM(E$23:F57)*$F$21*-1</f>
-        <v>1.8487991491247459E-6</v>
+        <v>4.6199999751083013E-11</v>
       </c>
       <c r="G58" s="23"/>
     </row>
@@ -3322,11 +3316,11 @@
       <c r="C59" s="21"/>
       <c r="D59" s="22">
         <f>E58*$E$22</f>
-        <v>1.2325327660831639E-6</v>
+        <v>3.0799999834055342E-11</v>
       </c>
       <c r="E59" s="21">
         <f>D58*$D$22</f>
-        <v>-1.2325327660831641E-6</v>
+        <v>1.3486265772649011E-25</v>
       </c>
       <c r="F59" s="22"/>
       <c r="G59" s="23">
@@ -3361,19 +3355,19 @@
       <c r="B61" s="16"/>
       <c r="C61" s="17">
         <f>SUM(C$23:D60)*$C$21*-1</f>
-        <v>-5.2822832832135608E-7</v>
+        <v>-1.3199999928880861E-11</v>
       </c>
       <c r="D61" s="18">
         <f>SUM(C$23:D60)*$D$21*-1</f>
-        <v>-7.0430443776180817E-7</v>
+        <v>-1.7599999905174483E-11</v>
       </c>
       <c r="E61" s="17">
         <f>SUM(E$23:F60)*$E$21*-1</f>
-        <v>7.0430443776180817E-7</v>
+        <v>-8.0757146435463234E-26</v>
       </c>
       <c r="F61" s="18">
         <f>SUM(E$23:F60)*$F$21*-1</f>
-        <v>5.2822832832135608E-7</v>
+        <v>-6.056785982659742E-26</v>
       </c>
       <c r="G61" s="19"/>
     </row>
@@ -3385,11 +3379,11 @@
       <c r="C62" s="17"/>
       <c r="D62" s="18">
         <f>E61*$E$22</f>
-        <v>3.5215221888090409E-7</v>
+        <v>-4.0378573217731617E-26</v>
       </c>
       <c r="E62" s="17">
         <f>D61*$D$22</f>
-        <v>-3.5215221888090409E-7</v>
+        <v>-8.7999999525872413E-12</v>
       </c>
       <c r="F62" s="18"/>
       <c r="G62" s="19">
@@ -3424,19 +3418,19 @@
       <c r="B64" s="20"/>
       <c r="C64" s="21">
         <f>SUM(C$23:D63)*$C$21*-1</f>
-        <v>-1.5092237952038751E-7</v>
+        <v>1.8689891779507237E-26</v>
       </c>
       <c r="D64" s="22">
         <f>SUM(C$23:D63)*$D$21*-1</f>
-        <v>-2.0122983936051666E-7</v>
+        <v>2.491985570600965E-26</v>
       </c>
       <c r="E64" s="21">
         <f>SUM(E$23:F63)*$E$21*-1</f>
-        <v>2.0122983936051666E-7</v>
+        <v>5.028571401478424E-12</v>
       </c>
       <c r="F64" s="22">
         <f>SUM(E$23:F63)*$F$21*-1</f>
-        <v>1.5092237952038751E-7</v>
+        <v>3.771428551108818E-12</v>
       </c>
       <c r="G64" s="23"/>
     </row>
@@ -3448,11 +3442,11 @@
       <c r="C65" s="21"/>
       <c r="D65" s="22">
         <f>E64*$E$22</f>
-        <v>1.0061491968025833E-7</v>
+        <v>2.514285700739212E-12</v>
       </c>
       <c r="E65" s="21">
         <f>D64*$D$22</f>
-        <v>-1.0061491968025833E-7</v>
+        <v>1.2459927853004825E-26</v>
       </c>
       <c r="F65" s="22"/>
       <c r="G65" s="23">
@@ -3487,19 +3481,19 @@
       <c r="B67" s="16"/>
       <c r="C67" s="17">
         <f>SUM(C$23:D66)*$C$21*-1</f>
-        <v>-4.3120679862967867E-8</v>
+        <v>-1.0775510146025196E-12</v>
       </c>
       <c r="D67" s="18">
         <f>SUM(C$23:D66)*$D$21*-1</f>
-        <v>-5.7494239817290489E-8</v>
+        <v>-1.4367346861366928E-12</v>
       </c>
       <c r="E67" s="17">
         <f>SUM(E$23:F66)*$E$21*-1</f>
-        <v>5.7494239817290489E-8</v>
+        <v>-7.5815550971149402E-27</v>
       </c>
       <c r="F67" s="18">
         <f>SUM(E$23:F66)*$F$21*-1</f>
-        <v>4.3120679862967867E-8</v>
+        <v>-5.6861663228362045E-27</v>
       </c>
       <c r="G67" s="19"/>
     </row>
@@ -3511,11 +3505,11 @@
       <c r="C68" s="17"/>
       <c r="D68" s="18">
         <f>E67*$E$22</f>
-        <v>2.8747119908645245E-8</v>
+        <v>-3.7907775485574701E-27</v>
       </c>
       <c r="E68" s="17">
         <f>D67*$D$22</f>
-        <v>-2.8747119908645245E-8</v>
+        <v>-7.1836734306834641E-13</v>
       </c>
       <c r="F68" s="18"/>
       <c r="G68" s="19">
@@ -3550,19 +3544,19 @@
       <c r="B70" s="20"/>
       <c r="C70" s="21">
         <f>SUM(C$23:D69)*$C$21*-1</f>
-        <v>-1.2320194246562248E-8</v>
+        <v>1.7977175708702694E-27</v>
       </c>
       <c r="D70" s="22">
         <f>SUM(C$23:D69)*$D$21*-1</f>
-        <v>-1.6426925662082997E-8</v>
+        <v>2.3969567611603591E-27</v>
       </c>
       <c r="E70" s="21">
         <f>SUM(E$23:F69)*$E$21*-1</f>
-        <v>1.6426925662082997E-8</v>
+        <v>4.1049562461048373E-13</v>
       </c>
       <c r="F70" s="22">
         <f>SUM(E$23:F69)*$F$21*-1</f>
-        <v>1.2320194246562248E-8</v>
+        <v>3.0787171845786278E-13</v>
       </c>
       <c r="G70" s="23"/>
     </row>
@@ -3574,11 +3568,11 @@
       <c r="C71" s="21"/>
       <c r="D71" s="22">
         <f>E70*$E$22</f>
-        <v>8.2134628310414984E-9</v>
+        <v>2.0524781230524186E-13</v>
       </c>
       <c r="E71" s="21">
         <f>D70*$D$22</f>
-        <v>-8.2134628310414984E-9</v>
+        <v>1.1984783805801796E-27</v>
       </c>
       <c r="F71" s="22"/>
       <c r="G71" s="23">
@@ -3613,19 +3607,19 @@
       <c r="B73" s="16"/>
       <c r="C73" s="17">
         <f>SUM(C$23:D72)*$C$21*-1</f>
-        <v>-3.5200554990177848E-9</v>
+        <v>-8.7963348130817954E-14</v>
       </c>
       <c r="D73" s="18">
         <f>SUM(C$23:D72)*$D$21*-1</f>
-        <v>-4.6934073320237128E-9</v>
+        <v>-1.1728446417442395E-13</v>
       </c>
       <c r="E73" s="17">
         <f>SUM(E$23:F72)*$E$21*-1</f>
-        <v>4.6934073320237128E-9</v>
+        <v>-7.4254432939912526E-28</v>
       </c>
       <c r="F73" s="18">
         <f>SUM(E$23:F72)*$F$21*-1</f>
-        <v>3.5200554990177848E-9</v>
+        <v>-5.569082470493439E-28</v>
       </c>
       <c r="G73" s="19"/>
     </row>
@@ -3637,11 +3631,11 @@
       <c r="C74" s="17"/>
       <c r="D74" s="18">
         <f>E73*$E$22</f>
-        <v>2.3467036660118564E-9</v>
+        <v>-3.7127216469956263E-28</v>
       </c>
       <c r="E74" s="17">
         <f>D73*$D$22</f>
-        <v>-2.3467036660118564E-9</v>
+        <v>-5.8642232087211973E-14</v>
       </c>
       <c r="F74" s="18"/>
       <c r="G74" s="19">
@@ -3676,19 +3670,19 @@
       <c r="B76" s="20"/>
       <c r="C76" s="21">
         <f>SUM(C$23:D75)*$C$21*-1</f>
-        <v>-1.0057301425765102E-9</v>
+        <v>1.6993530585712929E-28</v>
       </c>
       <c r="D76" s="22">
         <f>SUM(C$23:D75)*$D$21*-1</f>
-        <v>-1.340973523435347E-9</v>
+        <v>2.2658040780950576E-28</v>
       </c>
       <c r="E76" s="21">
         <f>SUM(E$23:F75)*$E$21*-1</f>
-        <v>1.340973523435347E-9</v>
+        <v>3.3509846906978276E-14</v>
       </c>
       <c r="F76" s="22">
         <f>SUM(E$23:F75)*$F$21*-1</f>
-        <v>1.0057301425765102E-9</v>
+        <v>2.5132385180233704E-14</v>
       </c>
       <c r="G76" s="23"/>
     </row>
@@ -3700,11 +3694,11 @@
       <c r="C77" s="21"/>
       <c r="D77" s="22">
         <f>E76*$E$22</f>
-        <v>6.7048676171767349E-10</v>
+        <v>1.6754923453489138E-14</v>
       </c>
       <c r="E77" s="21">
         <f>D76*$D$22</f>
-        <v>-6.7048676171767349E-10</v>
+        <v>1.1329020390475288E-28</v>
       </c>
       <c r="F77" s="22"/>
       <c r="G77" s="23">
@@ -3739,19 +3733,19 @@
       <c r="B79" s="16"/>
       <c r="C79" s="17">
         <f>SUM(C$23:D78)*$C$21*-1</f>
-        <v>-2.8735146930757432E-10</v>
+        <v>-7.1806814800667734E-15</v>
       </c>
       <c r="D79" s="18">
         <f>SUM(C$23:D78)*$D$21*-1</f>
-        <v>-3.8313529241009912E-10</v>
+        <v>-9.5742419734223661E-15</v>
       </c>
       <c r="E79" s="17">
         <f>SUM(E$23:F78)*$E$21*-1</f>
-        <v>3.8313529241009912E-10</v>
+        <v>-6.8343480655154848E-29</v>
       </c>
       <c r="F79" s="18">
         <f>SUM(E$23:F78)*$F$21*-1</f>
-        <v>2.8735146930757432E-10</v>
+        <v>-5.1257610491366136E-29</v>
       </c>
       <c r="G79" s="19"/>
     </row>
@@ -3763,11 +3757,11 @@
       <c r="C80" s="17"/>
       <c r="D80" s="18">
         <f>E79*$E$22</f>
-        <v>1.9156764620504956E-10</v>
+        <v>-3.4171740327577424E-29</v>
       </c>
       <c r="E80" s="17">
         <f>D79*$D$22</f>
-        <v>-1.9156764620504956E-10</v>
+        <v>-4.7871209867111831E-15</v>
       </c>
       <c r="F80" s="18"/>
       <c r="G80" s="19">
@@ -3802,19 +3796,19 @@
       <c r="B82" s="20"/>
       <c r="C82" s="21">
         <f>SUM(C$23:D81)*$C$21*-1</f>
-        <v>-8.2100419802164121E-11</v>
+        <v>1.5321198059151194E-29</v>
       </c>
       <c r="D82" s="22">
         <f>SUM(C$23:D81)*$D$21*-1</f>
-        <v>-1.0946722640288549E-10</v>
+        <v>2.0428264078868259E-29</v>
       </c>
       <c r="E82" s="21">
         <f>SUM(E$23:F81)*$E$21*-1</f>
-        <v>1.0946722640288549E-10</v>
+        <v>2.7354977066921051E-15</v>
       </c>
       <c r="F82" s="22">
         <f>SUM(E$23:F81)*$F$21*-1</f>
-        <v>8.2100419802164121E-11</v>
+        <v>2.0516232800190788E-15</v>
       </c>
       <c r="G82" s="23"/>
     </row>
@@ -3826,11 +3820,11 @@
       <c r="C83" s="25"/>
       <c r="D83" s="26">
         <f>E82*$E$22</f>
-        <v>5.4733613201442745E-11</v>
+        <v>1.3677488533460525E-15</v>
       </c>
       <c r="E83" s="25">
         <f>D82*$D$22</f>
-        <v>-5.4733613201442745E-11</v>
+        <v>1.021413203943413E-29</v>
       </c>
       <c r="F83" s="26"/>
       <c r="G83" s="27">
@@ -3845,19 +3839,19 @@
       </c>
       <c r="C84" s="31">
         <f t="shared" ref="C84:G84" si="3">SUM(C23:C83)</f>
-        <v>9.9960000000328399</v>
+        <v>5.5509328580574689E-5</v>
       </c>
       <c r="D84" s="31">
         <f t="shared" si="3"/>
-        <v>-9.9959999999781104</v>
+        <v>-5.5509328579206947E-5</v>
       </c>
       <c r="E84" s="31">
         <f t="shared" si="3"/>
-        <v>9.9959999999781104</v>
+        <v>-1.3877332144801735E-5</v>
       </c>
       <c r="F84" s="31">
         <f t="shared" si="3"/>
-        <v>-9.9960000000328399</v>
+        <v>1.3877332144801739E-5</v>
       </c>
       <c r="G84" s="32">
         <f t="shared" si="3"/>
@@ -4135,7 +4129,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4797,7 +4791,7 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="117">
+      <c r="C42" s="111">
         <f>SUM(C21:C31)</f>
         <v>0</v>
       </c>
@@ -4805,7 +4799,7 @@
         <f>SUM(D21:D31)</f>
         <v>12.499949999999998</v>
       </c>
-      <c r="E42" s="118">
+      <c r="E42" s="112">
         <f>SUM(E21:E31)</f>
         <v>-12.499949999999998</v>
       </c>
@@ -4832,15 +4826,17 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:U84"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4873,9 +4869,9 @@
       <c r="H3" s="71"/>
       <c r="I3" s="72"/>
       <c r="K3" s="39"/>
-      <c r="L3" s="116"/>
+      <c r="L3" s="110"/>
       <c r="M3" s="39"/>
-      <c r="N3" s="116"/>
+      <c r="N3" s="110"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -4895,7 +4891,7 @@
       <c r="G4" s="71"/>
       <c r="H4" s="71"/>
       <c r="I4" s="72"/>
-      <c r="J4" s="115"/>
+      <c r="J4" s="109"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
@@ -4914,7 +4910,7 @@
       <c r="G5" s="71"/>
       <c r="H5" s="71"/>
       <c r="I5" s="72"/>
-      <c r="J5" s="115"/>
+      <c r="J5" s="109"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -4932,7 +4928,7 @@
       <c r="G6" s="71"/>
       <c r="H6" s="71"/>
       <c r="I6" s="72"/>
-      <c r="J6" s="115"/>
+      <c r="J6" s="109"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="73"/>
@@ -4943,7 +4939,7 @@
       <c r="G7" s="71"/>
       <c r="H7" s="71"/>
       <c r="I7" s="72"/>
-      <c r="J7" s="115"/>
+      <c r="J7" s="109"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="104" t="s">
@@ -5075,7 +5071,7 @@
       <c r="H16" s="71"/>
       <c r="I16" s="72"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="104" t="s">
         <v>51</v>
       </c>
@@ -5094,7 +5090,7 @@
       <c r="H17" s="71"/>
       <c r="I17" s="72"/>
     </row>
-    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="93" t="s">
         <v>52</v>
       </c>
@@ -5113,8 +5109,8 @@
       <c r="H18" s="74"/>
       <c r="I18" s="75"/>
     </row>
-    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="76" t="s">
         <v>53</v>
       </c>
@@ -5131,18 +5127,22 @@
       </c>
       <c r="K20" s="95">
         <f t="shared" ref="K20:L20" si="0">G37</f>
-        <v>-6.6000000000000094</v>
+        <v>-8.3333333333333535</v>
       </c>
       <c r="L20" s="96" t="str">
         <f t="shared" si="0"/>
         <v>ft-kips</v>
       </c>
       <c r="O20">
-        <f>(0.4*C34)-(0.2*((0.5*C21*C21*C28)-(C21*C33)-(C36)))</f>
-        <v>-6.6000000000000094</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>((((C28*C21*C21)/2)-(C33*C21)-C36+(-2*C34))/(-0.5*C21))</f>
+        <v>-8.3333333333333535</v>
+      </c>
+      <c r="P20">
+        <f>K20/O20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="70" t="s">
         <v>37</v>
       </c>
@@ -5163,18 +5163,22 @@
       </c>
       <c r="K21" s="94">
         <f t="shared" ref="K21" si="1">G38</f>
-        <v>6.5999999999999961</v>
+        <v>8.3333333333333215</v>
       </c>
       <c r="L21" s="103" t="str">
         <f t="shared" ref="L21" si="2">H38</f>
         <v>ft-kips</v>
       </c>
       <c r="O21">
-        <f>(0.2*C34)-(0.4*((0.5*C21*C21*C28)-(C21*C33)-(C36)))</f>
-        <v>6.5999999999999961</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+        <f>(-1*C34+(O20*(C21/3)))/(C21/6)</f>
+        <v>8.3333333333333197</v>
+      </c>
+      <c r="P21">
+        <f>K21/O21</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="70" t="s">
         <v>54</v>
       </c>
@@ -5195,12 +5199,12 @@
       <c r="K22" s="71"/>
       <c r="L22" s="72"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="70" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="84">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" s="71" t="s">
         <v>1</v>
@@ -5216,12 +5220,12 @@
       <c r="K23" s="71"/>
       <c r="L23" s="72"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="70" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="84">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D24" s="71" t="s">
         <v>1</v>
@@ -5237,13 +5241,13 @@
       <c r="K24" s="71"/>
       <c r="L24" s="72"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="70" t="s">
         <v>61</v>
       </c>
       <c r="C25" s="9">
         <f>C24-C23</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D25" s="71" t="s">
         <v>1</v>
@@ -5259,7 +5263,7 @@
       <c r="K25" s="71"/>
       <c r="L25" s="72"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="73"/>
       <c r="C26" s="71"/>
       <c r="D26" s="71"/>
@@ -5272,13 +5276,13 @@
       <c r="K26" s="71"/>
       <c r="L26" s="72"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="70" t="s">
         <v>59</v>
       </c>
       <c r="C27" s="9">
         <f>(C22*C25)-(((C22*C25)*(C23+(C25/2)))/C21)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D27" s="71" t="s">
         <v>39</v>
@@ -5294,13 +5298,13 @@
       <c r="K27" s="71"/>
       <c r="L27" s="72"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
         <v>60</v>
       </c>
       <c r="C28" s="9">
         <f>(((C22*C25)*(C23+(C25/2)))/C21)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28" s="71" t="s">
         <v>39</v>
@@ -5316,7 +5320,7 @@
       <c r="K28" s="71"/>
       <c r="L28" s="72"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="73"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -5329,7 +5333,7 @@
       <c r="K29" s="71"/>
       <c r="L29" s="72"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="77" t="s">
         <v>63</v>
       </c>
@@ -5344,7 +5348,7 @@
       <c r="K30" s="71"/>
       <c r="L30" s="72"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="70" t="s">
         <v>64</v>
       </c>
@@ -5358,7 +5362,7 @@
       </c>
       <c r="G31" s="81">
         <f>C34*-1</f>
-        <v>33.000000000000021</v>
+        <v>41.666666666666714</v>
       </c>
       <c r="H31" s="71" t="s">
         <v>75</v>
@@ -5368,13 +5372,13 @@
       <c r="K31" s="71"/>
       <c r="L31" s="72"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="9">
         <f>((-1*C22*C23*C23)/2)</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D32" s="71"/>
       <c r="E32" s="71"/>
@@ -5383,7 +5387,7 @@
       </c>
       <c r="G32" s="82">
         <f>(((-1 * C28*C21*C21) / 2) + (C33 *C21) +C36)*-1</f>
-        <v>-33</v>
+        <v>-41.666666666666657</v>
       </c>
       <c r="H32" s="71" t="s">
         <v>76</v>
@@ -5399,7 +5403,7 @@
       </c>
       <c r="C33" s="9">
         <f>C28*C21</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D33" s="71"/>
       <c r="E33" s="71"/>
@@ -5417,18 +5421,18 @@
       </c>
       <c r="C34" s="9">
         <f>((C22*C23*C23*C23) / 3) + (C32*C23) +C35 - (C31*C23)</f>
-        <v>-33.000000000000021</v>
+        <v>-41.666666666666714</v>
       </c>
       <c r="D34" s="71"/>
       <c r="E34" s="71"/>
       <c r="F34" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="126">
+      <c r="G34" s="120">
         <f>(-1*C21)/3</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="H34" s="127">
+      <c r="H34" s="121">
         <f>C21/6</f>
         <v>1.6666666666666667</v>
       </c>
@@ -5445,18 +5449,18 @@
       </c>
       <c r="C35" s="9">
         <f>((-1*C27*C24*C24) / 2) + ((C22*POWER(C24,3)) / 6) - ((C22*C23*C24*C24) / 2) - ((C28*C24*C24) / 2) + (C33*C24) - (C32*C24) + C36</f>
-        <v>-31.666666666666686</v>
+        <v>-41.666666666666714</v>
       </c>
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
       <c r="F35" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="128">
+      <c r="G35" s="122">
         <f>C21/6</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="H35" s="129">
+      <c r="H35" s="123">
         <f>(-1*C21)/3</f>
         <v>-3.3333333333333335</v>
       </c>
@@ -5471,7 +5475,7 @@
       </c>
       <c r="C36" s="9">
         <f>((C28*C21*C21)/6)-((C33*C21)/2)-(C39/C21)</f>
-        <v>-117</v>
+        <v>-208.33333333333334</v>
       </c>
       <c r="D36" s="71"/>
       <c r="E36" s="71"/>
@@ -5497,7 +5501,7 @@
       </c>
       <c r="G37" s="88" cm="1">
         <f t="array" ref="G37:G38">MMULT(MINVERSE(G34:H35),G31:G32)</f>
-        <v>-6.6000000000000094</v>
+        <v>-8.3333333333333535</v>
       </c>
       <c r="H37" s="89" t="s">
         <v>46</v>
@@ -5515,7 +5519,7 @@
       </c>
       <c r="C38" s="9">
         <f>((-1*C31*C23*C23)/2)+((C32*C23*C23)/2)+((5*C22*POWER(C23,4))/24)+C37</f>
-        <v>-0.66666666666666652</v>
+        <v>0</v>
       </c>
       <c r="D38" s="71"/>
       <c r="E38" s="71"/>
@@ -5523,7 +5527,7 @@
         <v>52</v>
       </c>
       <c r="G38" s="91">
-        <v>6.5999999999999961</v>
+        <v>8.3333333333333215</v>
       </c>
       <c r="H38" s="92" t="s">
         <v>46</v>
@@ -5541,7 +5545,7 @@
       </c>
       <c r="C39" s="9">
         <f>((-1*C27*POWER(C24,3))/3)-((C28*POWER(C24,3))/3)+((C22*POWER(C24,4))/8)-((C22*C23*POWER(C24,3))/3)-((C32*C24*C24)/2)+((C33*C24*C24)/2)+C38</f>
-        <v>170.00000000000009</v>
+        <v>416.66666666666652</v>
       </c>
       <c r="D39" s="71"/>
       <c r="E39" s="71"/>
@@ -5587,15 +5591,19 @@
       </c>
       <c r="N42" s="95">
         <f t="shared" ref="N42:O42" si="3">F64</f>
-        <v>-5.2440000000000042</v>
+        <v>-0.13333333333333341</v>
       </c>
       <c r="O42" s="96" t="str">
         <f t="shared" si="3"/>
         <v>ft-kips</v>
       </c>
       <c r="R42">
-        <f>(0.4*C61)-(0.2*((0.5*C43*C43*C55)-(C43*C60)-(C63)))</f>
-        <v>-5.2440000000000042</v>
+        <f>((((C55*C43*C43)/2)-(C60*C43)-C63+(-2*C61))/(-0.5*C43))</f>
+        <v>-0.13333333333333341</v>
+      </c>
+      <c r="S42">
+        <f>N42/R42</f>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5603,7 +5611,7 @@
         <v>37</v>
       </c>
       <c r="C43" s="84">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D43" s="71" t="s">
         <v>1</v>
@@ -5624,15 +5632,19 @@
       </c>
       <c r="N43" s="94">
         <f t="shared" ref="N43" si="4">F65</f>
-        <v>4.6559999999999997</v>
+        <v>0.2</v>
       </c>
       <c r="O43" s="103" t="str">
         <f t="shared" ref="O43" si="5">G65</f>
         <v>ft-kips</v>
       </c>
       <c r="R43">
-        <f>(0.2*C61)-(0.4*((0.5*C43*C43*C55)-(C43*C60)-(C63)))</f>
-        <v>4.6559999999999997</v>
+        <f>(-1*C61+(R42*(C43/3)))/(C43/6)</f>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="S43">
+        <f>N43/R43</f>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.25">
@@ -5640,7 +5652,7 @@
         <v>83</v>
       </c>
       <c r="C44" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="71" t="s">
         <v>56</v>
@@ -5669,7 +5681,7 @@
         <v>84</v>
       </c>
       <c r="C45" s="84">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D45" s="71" t="s">
         <v>56</v>
@@ -5699,7 +5711,7 @@
         <v>40</v>
       </c>
       <c r="C46" s="84">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D46" s="71" t="s">
         <v>1</v>
@@ -5729,7 +5741,7 @@
         <v>55</v>
       </c>
       <c r="C47" s="84">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D47" s="71" t="s">
         <v>1</v>
@@ -5760,7 +5772,7 @@
       </c>
       <c r="C48" s="9">
         <f>C47-C46</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D48" s="71" t="s">
         <v>1</v>
@@ -5812,7 +5824,7 @@
       </c>
       <c r="C50" s="9">
         <f>(C45-C44)/C48</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>0.5</v>
       </c>
       <c r="D50" s="71" t="s">
         <v>89</v>
@@ -5836,7 +5848,7 @@
       </c>
       <c r="C51" s="9">
         <f>(C48* ((2 *C45) + C44)) / (3 * (C45+ C44))</f>
-        <v>2.6666666666666665</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="D51" s="71" t="s">
         <v>91</v>
@@ -5860,7 +5872,7 @@
       </c>
       <c r="C52" s="9">
         <f>C48 * ((C44 + C45) / 2)</f>
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="D52" s="71" t="s">
         <v>93</v>
@@ -5901,7 +5913,7 @@
       </c>
       <c r="C54" s="86">
         <f>C52-C55</f>
-        <v>2.4000000000000004</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="D54" s="71" t="s">
         <v>39</v>
@@ -5931,7 +5943,7 @@
       </c>
       <c r="C55" s="86">
         <f>(C52* (C46 +C51)) / C43</f>
-        <v>2.0999999999999996</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D55" s="71" t="s">
         <v>39</v>
@@ -5991,7 +6003,7 @@
       <c r="B58" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="130">
+      <c r="C58" s="124">
         <v>0</v>
       </c>
       <c r="D58" s="71"/>
@@ -6000,7 +6012,7 @@
       </c>
       <c r="F58" s="81">
         <f>C61*-1</f>
-        <v>25.240000000000013</v>
+        <v>0.15555555555555561</v>
       </c>
       <c r="G58" s="71" t="s">
         <v>75</v>
@@ -6019,9 +6031,9 @@
       <c r="B59" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="130">
+      <c r="C59" s="124">
         <f>C58 + ((POWER(C46,3) * C50) / 6) + ((C46*C46* (C44 - (C50 * C46))) / 2) + ((((C50 * C46) - (2 * C44)) * C46*C46) / 2)</f>
-        <v>-2.1111111111111107</v>
+        <v>0</v>
       </c>
       <c r="D59" s="71"/>
       <c r="E59" s="78" t="s">
@@ -6029,7 +6041,7 @@
       </c>
       <c r="F59" s="82">
         <f>(((-1 * C55 * C43*C43) / 2) + (C60 * C43) + C63)*-1</f>
-        <v>-24.260000000000005</v>
+        <v>-0.17777777777777781</v>
       </c>
       <c r="G59" s="71" t="s">
         <v>76</v>
@@ -6047,9 +6059,9 @@
       <c r="B60" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="130">
+      <c r="C60" s="124">
         <f>C55*C43</f>
-        <v>20.999999999999996</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="D60" s="71"/>
       <c r="E60" s="71"/>
@@ -6068,21 +6080,21 @@
       <c r="B61" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="130">
+      <c r="C61" s="124">
         <f>((-1 * POWER(C46,4) *C50) / 24) - ((POWER(C46,3) * (C44 - (C50 * C46))) / 6) - ((((C50 * C46) - (2 * C44)) * POWER(C46,3)) / 4) + (C59* C46) + C62 - (C58 * C46)</f>
-        <v>-25.240000000000013</v>
+        <v>-0.15555555555555561</v>
       </c>
       <c r="D61" s="71"/>
       <c r="E61" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="F61" s="126">
+      <c r="F61" s="120">
         <f>(-1*C43)/3</f>
-        <v>-3.3333333333333335</v>
-      </c>
-      <c r="G61" s="127">
+        <v>-0.66666666666666663</v>
+      </c>
+      <c r="G61" s="121">
         <f>C43/6</f>
-        <v>1.6666666666666667</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H61" s="71" t="s">
         <v>81</v>
@@ -6099,21 +6111,21 @@
       <c r="B62" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="130">
+      <c r="C62" s="124">
         <f>((-1 * C55 * C47*C47) / 2) + (C60 *C47) + C63 - ((C54 * C47*C47) / 2) + ((POWER(C47,4) *C50) / 24) + ((POWER(C47,3)* (C44 - (C50 * C46))) / 6) + ((((C50 * C46) - (2 * C44)) *C46 *C47*C47) / 4) - (C59 * C47)</f>
-        <v>-23.851111111111123</v>
+        <v>-0.15555555555555561</v>
       </c>
       <c r="D62" s="71"/>
       <c r="E62" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="F62" s="128">
+      <c r="F62" s="122">
         <f>C43/6</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G62" s="129">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G62" s="123">
         <f>(-1*C43)/3</f>
-        <v>-3.3333333333333335</v>
+        <v>-0.66666666666666663</v>
       </c>
       <c r="H62" s="71"/>
       <c r="I62" s="71"/>
@@ -6128,9 +6140,9 @@
       <c r="B63" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="130">
+      <c r="C63" s="124">
         <f>(((C55 * C43*C43*C43) / 6) - ((C60 * C43*C43) / 2) - C66) / C43</f>
-        <v>-80.739999999999981</v>
+        <v>-1.1555555555555554</v>
       </c>
       <c r="D63" s="71"/>
       <c r="E63" s="71"/>
@@ -6149,7 +6161,7 @@
       <c r="B64" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="130">
+      <c r="C64" s="124">
         <v>0</v>
       </c>
       <c r="D64" s="71"/>
@@ -6158,7 +6170,7 @@
       </c>
       <c r="F64" s="88" cm="1">
         <f t="array" ref="F64:F65">MMULT(MINVERSE(F61:G62),F58:F59)</f>
-        <v>-5.2440000000000042</v>
+        <v>-0.13333333333333341</v>
       </c>
       <c r="G64" s="89" t="s">
         <v>46</v>
@@ -6178,16 +6190,16 @@
       <c r="B65" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="130">
+      <c r="C65" s="124">
         <f>((-1 * C58 * C46*C46) / 2) - ((POWER(C46,5) *C50) / 30) - ((POWER(C46,4) * (C44 - (C50 * C46))) / 8) - ((((C50 * C46) - (2 * C44)) * POWER(C46,4)) / 6) + ((C59 * C46*C46) / 2) + C64</f>
-        <v>-0.68888888888888822</v>
+        <v>0</v>
       </c>
       <c r="D65" s="71"/>
       <c r="E65" s="90" t="s">
         <v>52</v>
       </c>
       <c r="F65" s="91">
-        <v>4.6559999999999997</v>
+        <v>0.2</v>
       </c>
       <c r="G65" s="92" t="s">
         <v>46</v>
@@ -6207,9 +6219,9 @@
       <c r="B66" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="130">
+      <c r="C66" s="124">
         <f>((-1 * C54* POWER(C47,3)) / 3) + ((POWER(C47,5)* C50) / 30) + ((POWER(C47, 4) * (C44 - (C50 * C46))) / 8) + ((((C50 * C46) - (2 * C44)) * C46 * POWER(C47,3)) / 6) - ((C59 *C47*C47) / 2) + C65 - ((C55* POWER(C47,3)) / 3) + ((C60 * C47*C47) / 2)</f>
-        <v>107.39999999999998</v>
+        <v>0.53333333333333321</v>
       </c>
       <c r="D66" s="71"/>
       <c r="E66" s="71"/>
@@ -6250,13 +6262,16 @@
       <c r="E69" s="68"/>
       <c r="F69" s="68"/>
       <c r="G69" s="68"/>
-      <c r="H69" s="69"/>
+      <c r="H69" s="68"/>
+      <c r="I69" s="68"/>
+      <c r="J69" s="68"/>
+      <c r="K69" s="69"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="C70" s="110">
+      <c r="C70" s="106">
         <v>10</v>
       </c>
       <c r="D70" s="71" t="s">
@@ -6264,48 +6279,82 @@
       </c>
       <c r="E70" s="71"/>
       <c r="F70" s="71"/>
-      <c r="G70" s="71"/>
-      <c r="H70" s="72"/>
+      <c r="G70" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="H70" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="I70" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="J70" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="K70" s="72"/>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="C71" s="110">
-        <v>0</v>
-      </c>
-      <c r="D71" s="113" t="s">
-        <v>98</v>
-      </c>
-      <c r="E71" s="114">
+      <c r="C71" s="106">
+        <v>0</v>
+      </c>
+      <c r="D71" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="E71" s="108">
         <f>C71/12</f>
         <v>0</v>
       </c>
       <c r="F71" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G71" s="71"/>
-      <c r="H71" s="72"/>
+      <c r="G71" s="106">
+        <v>1</v>
+      </c>
+      <c r="H71" s="106">
+        <v>1</v>
+      </c>
+      <c r="I71" s="39">
+        <f>G71*144</f>
+        <v>144</v>
+      </c>
+      <c r="J71" s="71">
+        <f>H71/POWER(12,4)</f>
+        <v>4.8225308641975306E-5</v>
+      </c>
+      <c r="K71" s="72"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="C72" s="110">
-        <v>12</v>
-      </c>
-      <c r="D72" s="113" t="s">
-        <v>98</v>
-      </c>
-      <c r="E72" s="114">
+      <c r="C72" s="106">
+        <v>3</v>
+      </c>
+      <c r="D72" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="E72" s="108">
         <f>C72/12</f>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="F72" s="71" t="s">
         <v>1</v>
       </c>
       <c r="G72" s="71"/>
-      <c r="H72" s="72"/>
+      <c r="H72" s="71"/>
+      <c r="I72" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="J72" s="71">
+        <f>I71*J71</f>
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="K72" s="72" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73" s="73"/>
@@ -6314,23 +6363,29 @@
       <c r="E73" s="71"/>
       <c r="F73" s="71"/>
       <c r="G73" s="71"/>
-      <c r="H73" s="72"/>
+      <c r="H73" s="71"/>
+      <c r="I73" s="71"/>
+      <c r="J73" s="71"/>
+      <c r="K73" s="72"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B74" s="99" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C74" s="39">
-        <f>(E72-E71)/C70</f>
-        <v>0.1</v>
+        <f>((E72-E71)/C70)*J72</f>
+        <v>1.7361111111111112E-4</v>
       </c>
       <c r="D74" s="80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E74" s="71"/>
       <c r="F74" s="71"/>
       <c r="G74" s="71"/>
-      <c r="H74" s="72"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="71"/>
+      <c r="J74" s="71"/>
+      <c r="K74" s="72"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B75" s="73"/>
@@ -6339,15 +6394,18 @@
       <c r="E75" s="71"/>
       <c r="F75" s="71"/>
       <c r="G75" s="71"/>
-      <c r="H75" s="72"/>
+      <c r="H75" s="71"/>
+      <c r="I75" s="71"/>
+      <c r="J75" s="71"/>
+      <c r="K75" s="72"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="81">
+        <v>125</v>
+      </c>
+      <c r="C76" s="138">
         <f>-1*C74</f>
-        <v>-0.1</v>
+        <v>-1.7361111111111112E-4</v>
       </c>
       <c r="D76" s="71" t="s">
         <v>75</v>
@@ -6355,15 +6413,18 @@
       <c r="E76" s="71"/>
       <c r="F76" s="71"/>
       <c r="G76" s="71"/>
-      <c r="H76" s="72"/>
+      <c r="H76" s="71"/>
+      <c r="I76" s="71"/>
+      <c r="J76" s="71"/>
+      <c r="K76" s="72"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" s="82">
+        <v>126</v>
+      </c>
+      <c r="C77" s="138">
         <f>-1*C74</f>
-        <v>-0.1</v>
+        <v>-1.7361111111111112E-4</v>
       </c>
       <c r="D77" s="71" t="s">
         <v>76</v>
@@ -6371,7 +6432,10 @@
       <c r="E77" s="71"/>
       <c r="F77" s="71"/>
       <c r="G77" s="71"/>
-      <c r="H77" s="72"/>
+      <c r="H77" s="71"/>
+      <c r="I77" s="71"/>
+      <c r="J77" s="71"/>
+      <c r="K77" s="72"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="73"/>
@@ -6380,18 +6444,21 @@
       <c r="E78" s="71"/>
       <c r="F78" s="71"/>
       <c r="G78" s="71"/>
-      <c r="H78" s="72"/>
+      <c r="H78" s="71"/>
+      <c r="I78" s="71"/>
+      <c r="J78" s="71"/>
+      <c r="K78" s="72"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C79" s="106">
-        <f>(-1*C70)/3</f>
+        <v>127</v>
+      </c>
+      <c r="C79" s="86">
+        <f>(-1*C70)/(3)</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="D79" s="107">
-        <f>C70/6</f>
+      <c r="D79" s="86">
+        <f>C70/(6)</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="E79" s="71" t="s">
@@ -6399,43 +6466,52 @@
       </c>
       <c r="F79" s="71"/>
       <c r="G79" s="71"/>
-      <c r="H79" s="72"/>
+      <c r="H79" s="71"/>
+      <c r="I79" s="71"/>
+      <c r="J79" s="71"/>
+      <c r="K79" s="72"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="C80" s="108">
-        <f>C70/6</f>
+        <v>128</v>
+      </c>
+      <c r="C80" s="86">
+        <f>C70/(6)</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="D80" s="109">
-        <f>(-1*C70)/3</f>
+      <c r="D80" s="86">
+        <f>(-1*C70)/(3)</f>
         <v>-3.3333333333333335</v>
       </c>
       <c r="E80" s="71"/>
       <c r="F80" s="71"/>
       <c r="G80" s="71"/>
-      <c r="H80" s="72"/>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H80" s="71"/>
+      <c r="I80" s="71"/>
+      <c r="J80" s="71"/>
+      <c r="K80" s="72"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" s="73"/>
       <c r="C81" s="71"/>
       <c r="D81" s="71"/>
       <c r="E81" s="71"/>
       <c r="F81" s="71"/>
       <c r="G81" s="71"/>
-      <c r="H81" s="72"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="111" t="s">
+      <c r="H81" s="71"/>
+      <c r="I81" s="71"/>
+      <c r="J81" s="71"/>
+      <c r="K81" s="72"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="141" t="s">
         <v>51</v>
       </c>
-      <c r="C82" s="88" cm="1">
+      <c r="C82" s="139" cm="1">
         <f t="array" ref="C82:C83">MMULT(MINVERSE(C79:D80),C76:C77)</f>
-        <v>6.0000000000000012E-2</v>
-      </c>
-      <c r="D82" s="89" t="s">
+        <v>1.0416666666666666E-4</v>
+      </c>
+      <c r="D82" s="140" t="s">
         <v>46</v>
       </c>
       <c r="E82" s="71" t="s">
@@ -6443,16 +6519,22 @@
       </c>
       <c r="F82" s="71"/>
       <c r="G82" s="71"/>
-      <c r="H82" s="72"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="112" t="s">
+      <c r="H82" s="71"/>
+      <c r="I82" s="143">
+        <f>(6*J72*E72)/(C70*C70)</f>
+        <v>1.0416666666666666E-4</v>
+      </c>
+      <c r="J82" s="71"/>
+      <c r="K82" s="72"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="141" t="s">
         <v>52</v>
       </c>
-      <c r="C83" s="91">
-        <v>6.0000000000000012E-2</v>
-      </c>
-      <c r="D83" s="92" t="s">
+      <c r="C83" s="139">
+        <v>1.0416666666666666E-4</v>
+      </c>
+      <c r="D83" s="140" t="s">
         <v>46</v>
       </c>
       <c r="E83" s="71" t="s">
@@ -6460,16 +6542,22 @@
       </c>
       <c r="F83" s="71"/>
       <c r="G83" s="71"/>
-      <c r="H83" s="72"/>
-    </row>
-    <row r="84" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H83" s="71"/>
+      <c r="I83" s="71"/>
+      <c r="J83" s="71"/>
+      <c r="K83" s="72"/>
+    </row>
+    <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="79"/>
       <c r="C84" s="74"/>
       <c r="D84" s="74"/>
       <c r="E84" s="74"/>
       <c r="F84" s="74"/>
       <c r="G84" s="74"/>
-      <c r="H84" s="75"/>
+      <c r="H84" s="74"/>
+      <c r="I84" s="74"/>
+      <c r="J84" s="74"/>
+      <c r="K84" s="75"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>